<commit_message>
make Person the tree root
</commit_message>
<xml_diff>
--- a/project/excel/linkml_tutorial.xlsx
+++ b/project/excel/linkml_tutorial.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="9" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Animal" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AnimalCollection" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PersonCollection" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Animal1" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AnimalCollection1" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing1" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person1" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PersonCollection1" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Animal" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="AnimalCollection" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="NamedThing" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Person" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="PersonCollection" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Animal1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="AnimalCollection1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="NamedThing1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Person1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="PersonCollection1" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>